<commit_message>
feat: 🎸 add error handle
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/FILE/AW/STYLISH-main-project-1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/FILE/AW/STYLISH-main-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9114DE81-F622-FF4E-B147-F37C0A4E724B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A197F1-6A60-3146-B02A-EDC6E339B120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{2DC67D53-5B43-9248-8A7F-ED0747702EE2}"/>
   </bookViews>
@@ -47,113 +47,113 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>women</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>price</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>texture</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wash</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>note</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>story</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sizes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>place</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>厚薄：薄；彈性：無</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>棉 100%</t>
+  </si>
+  <si>
+    <t>手洗，溫水</t>
+  </si>
+  <si>
+    <t>中國</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>實品顏色依單品照為主</t>
+  </si>
+  <si>
+    <t>O.N.S is all about options, which is why we took our staple polo shirt and upgraded it with slubby linen jersey, making it even lighter for those who prefer their summer style extra-breezy.</t>
+  </si>
+  <si>
+    <t>https://images.pexels.com/photos/991511/pexels-photo-991511.jpeg?auto=compress&amp;cs=tinysrgb&amp;w=1260&amp;h=750&amp;dpr=1</t>
+  </si>
+  <si>
+    <t>https://images.pexels.com/photos/1021709/pexels-photo-1021709.jpeg?auto=compress&amp;cs=tinysrgb&amp;w=1260&amp;h=750&amp;dpr=1</t>
+  </si>
+  <si>
+    <t>S,M</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M,L</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>color_ids</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>other_images</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>main_image</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.pexels.com/photos/991509/pexels-photo-991509.jpeg?auto=compress&amp;cs=tinysrgb&amp;w=1260&amp;h=750&amp;dpr=1,https://plus.unsplash.com/premium_photo-1661693822833-3f1c4a876171?ixlib=rb-4.0.3&amp;ixid=MnwxMjA3fDB8MHxwaG90by1wYWdlfHx8fGVufDB8fHx8&amp;auto=format&amp;fit=crop&amp;w=1470&amp;q=80</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.pexels.com/photos/2173357/pexels-photo-2173357.jpeg?auto=compress&amp;cs=tinysrgb&amp;w=1260&amp;h=750&amp;dpr=1,https://images.unsplash.com/photo-1496747611176-843222e1e57c?ixlib=rb-4.0.3&amp;ixid=MnwxMjA3fDB8MHxwaG90by1wYWdlfHx8fGVufDB8fHx8&amp;auto=format&amp;fit=crop&amp;w=1473&amp;q=80</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>men</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>shirt</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>women</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dress</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>price</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>texture</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>wash</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>note</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>story</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sizes</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>place</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>厚薄：薄；彈性：無</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>棉 100%</t>
-  </si>
-  <si>
-    <t>手洗，溫水</t>
-  </si>
-  <si>
-    <t>中國</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>實品顏色依單品照為主</t>
-  </si>
-  <si>
-    <t>O.N.S is all about options, which is why we took our staple polo shirt and upgraded it with slubby linen jersey, making it even lighter for those who prefer their summer style extra-breezy.</t>
-  </si>
-  <si>
-    <t>https://images.pexels.com/photos/991511/pexels-photo-991511.jpeg?auto=compress&amp;cs=tinysrgb&amp;w=1260&amp;h=750&amp;dpr=1</t>
-  </si>
-  <si>
-    <t>https://images.pexels.com/photos/1021709/pexels-photo-1021709.jpeg?auto=compress&amp;cs=tinysrgb&amp;w=1260&amp;h=750&amp;dpr=1</t>
-  </si>
-  <si>
-    <t>S,M</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>M,L</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1,2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>color_ids</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>other_images</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>main_image</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>product_id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2,3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://images.pexels.com/photos/991509/pexels-photo-991509.jpeg?auto=compress&amp;cs=tinysrgb&amp;w=1260&amp;h=750&amp;dpr=1,https://plus.unsplash.com/premium_photo-1661693822833-3f1c4a876171?ixlib=rb-4.0.3&amp;ixid=MnwxMjA3fDB8MHxwaG90by1wYWdlfHx8fGVufDB8fHx8&amp;auto=format&amp;fit=crop&amp;w=1470&amp;q=80</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://images.pexels.com/photos/2173357/pexels-photo-2173357.jpeg?auto=compress&amp;cs=tinysrgb&amp;w=1260&amp;h=750&amp;dpr=1,https://images.unsplash.com/photo-1496747611176-843222e1e57c?ixlib=rb-4.0.3&amp;ixid=MnwxMjA3fDB8MHxwaG90by1wYWdlfHx8fGVufDB8fHx8&amp;auto=format&amp;fit=crop&amp;w=1473&amp;q=80</t>
+    <t>2,13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>另一個裙子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>襯衫</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -560,7 +560,7 @@
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -575,7 +575,7 @@
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -587,122 +587,122 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="N1" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2">
+        <v>30</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
         <v>14</v>
       </c>
-      <c r="E2">
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" t="s">
-        <v>20</v>
-      </c>
-      <c r="L2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M2" t="s">
-        <v>22</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="16" customHeight="1">
       <c r="A3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E3">
         <v>75</v>
       </c>
       <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" t="s">
         <v>15</v>
       </c>
-      <c r="G3" t="s">
+      <c r="J3" t="s">
         <v>16</v>
       </c>
-      <c r="H3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>18</v>
-      </c>
-      <c r="J3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3" t="s">
-        <v>21</v>
       </c>
       <c r="L3" t="s">
         <v>29</v>
       </c>
       <c r="M3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:14">

</xml_diff>